<commit_message>
Atualização do diário de Engenharia de Software II
- Atualização do diário de Engenharia de Software II
</commit_message>
<xml_diff>
--- a/Doc/Eng. Software II/EngSoftwareDiárioTodos.xlsx
+++ b/Doc/Eng. Software II/EngSoftwareDiárioTodos.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18528"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\GitHub\Trails4Health\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Fiuza Sanches\Documents\GitHub\Trails4Health\Doc\Eng. Software II\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20085" windowHeight="7410" xr2:uid="{E3483F1B-F5CC-4CDE-8702-5566078582CA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20088" windowHeight="7416" xr2:uid="{E3483F1B-F5CC-4CDE-8702-5566078582CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>Aula</t>
   </si>
@@ -67,6 +67,12 @@
   </si>
   <si>
     <t>Engenharia de Software II</t>
+  </si>
+  <si>
+    <t>5º Entrega</t>
+  </si>
+  <si>
+    <t>6º Entrega</t>
   </si>
 </sst>
 </file>
@@ -280,14 +286,8 @@
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -298,12 +298,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="20" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -313,23 +307,35 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -647,235 +653,264 @@
   <dimension ref="A1:J25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="N18" sqref="N18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="1" max="1" width="19.5546875" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" customWidth="1"/>
+    <col min="3" max="3" width="13.5546875" customWidth="1"/>
     <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="7" max="7" width="12.5703125" customWidth="1"/>
+    <col min="7" max="7" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-    </row>
-    <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
+    </row>
+    <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="4"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
-    </row>
-    <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="B2" s="20"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+    </row>
+    <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-    </row>
-    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="C3" s="4"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+    </row>
+    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="25">
+      <c r="B4" s="17">
         <v>1011713</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-    </row>
-    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="C4" s="4"/>
+      <c r="D4" s="3"/>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3"/>
+    </row>
+    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="25">
+      <c r="B5" s="17">
         <v>1012063</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-    </row>
-    <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="26" t="s">
+      <c r="C5" s="4"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
+      <c r="G5" s="3"/>
+    </row>
+    <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="13">
         <v>1012180</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-    </row>
-    <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-    </row>
-    <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-    </row>
-    <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-    </row>
-    <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
+    </row>
+    <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+    </row>
+    <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="22"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="3"/>
+      <c r="F8" s="3"/>
+      <c r="G8" s="3"/>
+    </row>
+    <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+    </row>
+    <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="19" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="20"/>
-      <c r="C10" s="21"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18"/>
-      <c r="B11" s="9" t="s">
+      <c r="B10" s="26"/>
+      <c r="C10" s="20"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+    </row>
+    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="21"/>
+      <c r="B11" s="24" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="7"/>
-    </row>
-    <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="18"/>
-      <c r="B12" s="11" t="s">
+      <c r="C11" s="25"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="21"/>
+      <c r="B12" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
-    </row>
-    <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="14">
+      <c r="B13" s="10">
         <v>6.25E-2</v>
       </c>
-      <c r="C13" s="15">
+      <c r="C13" s="11">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-    </row>
-    <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="10">
         <v>6.25E-2</v>
       </c>
-      <c r="C14" s="15">
+      <c r="C14" s="11">
         <v>0.16666666666666666</v>
       </c>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="10">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="C15" s="11">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="12" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="10">
         <v>6.25E-2</v>
       </c>
-      <c r="C15" s="15">
+      <c r="C16" s="11">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
+    </row>
+    <row r="17" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="10">
+        <v>6.25E-2</v>
+      </c>
+      <c r="C17" s="11">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16" s="14">
-        <v>6.25E-2</v>
-      </c>
-      <c r="C16" s="15">
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+    </row>
+    <row r="18" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A18" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="10">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
-    </row>
-    <row r="17" spans="3:10" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="11">
+        <v>0.1875</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C19" s="1"/>
     </row>
-    <row r="20" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="C20" s="1"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-    </row>
-    <row r="22" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="I20" s="23"/>
+      <c r="J20" s="23"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H22" s="1"/>
       <c r="I22" s="2"/>
       <c r="J22" s="2"/>
     </row>
-    <row r="23" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H23" s="1"/>
       <c r="I23" s="2"/>
       <c r="J23" s="2"/>
     </row>
-    <row r="24" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H24" s="1"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
     </row>
-    <row r="25" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
       <c r="H25" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Atualização dos diários de ambas as disciplinas pela aluna Andreia Ernesto.
</commit_message>
<xml_diff>
--- a/Doc/Eng. Software II/EngSoftwareDiárioTodos.xlsx
+++ b/Doc/Eng. Software II/EngSoftwareDiárioTodos.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Fiuza Sanches\Documents\GitHub\Trails4Health\Doc\Eng. Software II\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Acer\Documents\GitHub\Trails4Health\Doc\Eng. Software II\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20088" windowHeight="7416" xr2:uid="{E3483F1B-F5CC-4CDE-8702-5566078582CA}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20085" windowHeight="7410"/>
   </bookViews>
   <sheets>
     <sheet name="Folha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>Aula</t>
   </si>
@@ -73,12 +73,21 @@
   </si>
   <si>
     <t>6º Entrega</t>
+  </si>
+  <si>
+    <t>Descrição</t>
+  </si>
+  <si>
+    <t>7º Entrega</t>
+  </si>
+  <si>
+    <t>Atualização dos casos de uso e diagrama de estados</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -148,7 +157,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -276,11 +285,107 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
@@ -305,7 +410,6 @@
     <xf numFmtId="20" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
@@ -335,6 +439,38 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -649,93 +785,99 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1721EC4-4771-467E-9FB1-874291366E44}">
-  <dimension ref="A1:J25"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="19.5546875" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="13.5546875" customWidth="1"/>
-    <col min="5" max="5" width="15" customWidth="1"/>
-    <col min="7" max="7" width="12.5546875" customWidth="1"/>
+    <col min="1" max="1" width="19.5703125" customWidth="1"/>
+    <col min="2" max="2" width="30.85546875" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" customWidth="1"/>
+    <col min="6" max="6" width="15" customWidth="1"/>
+    <col min="8" max="8" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C1" s="3"/>
+    <row r="1" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
-    </row>
-    <row r="2" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="H1" s="3"/>
+    </row>
+    <row r="2" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="20"/>
-      <c r="C2" s="3"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="19"/>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-    </row>
-    <row r="3" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="H2" s="3"/>
+    </row>
+    <row r="3" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="27"/>
+      <c r="C3" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="D3" s="3"/>
+      <c r="D3" s="4"/>
       <c r="E3" s="3"/>
       <c r="F3" s="3"/>
       <c r="G3" s="3"/>
-    </row>
-    <row r="4" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="16" t="s">
+      <c r="H3" s="3"/>
+    </row>
+    <row r="4" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="28"/>
+      <c r="C4" s="16">
         <v>1011713</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="3"/>
+      <c r="D4" s="4"/>
       <c r="E4" s="3"/>
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
-    </row>
-    <row r="5" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="16" t="s">
+      <c r="H4" s="3"/>
+    </row>
+    <row r="5" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="28"/>
+      <c r="C5" s="16">
         <v>1012063</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="3"/>
+      <c r="D5" s="4"/>
       <c r="E5" s="3"/>
       <c r="F5" s="3"/>
       <c r="G5" s="3"/>
-    </row>
-    <row r="6" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="18" t="s">
+      <c r="H5" s="3"/>
+    </row>
+    <row r="6" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="29"/>
+      <c r="C6" s="12">
         <v>1012180</v>
       </c>
-      <c r="C6" s="3"/>
       <c r="D6" s="3"/>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3"/>
-    </row>
-    <row r="7" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H6" s="3"/>
+    </row>
+    <row r="7" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
@@ -743,17 +885,19 @@
       <c r="E7" s="3"/>
       <c r="F7" s="3"/>
       <c r="G7" s="3"/>
-    </row>
-    <row r="8" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H7" s="3"/>
+    </row>
+    <row r="8" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3"/>
-      <c r="C8" s="22"/>
-      <c r="D8" s="22"/>
-      <c r="E8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
       <c r="F8" s="3"/>
       <c r="G8" s="3"/>
-    </row>
-    <row r="9" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H8" s="3"/>
+    </row>
+    <row r="9" spans="1:8" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -761,166 +905,197 @@
       <c r="E9" s="3"/>
       <c r="F9" s="3"/>
       <c r="G9" s="3"/>
-    </row>
-    <row r="10" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="19" t="s">
+      <c r="H9" s="3"/>
+    </row>
+    <row r="10" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="26"/>
-      <c r="C10" s="20"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="6"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="25"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="3"/>
       <c r="F10" s="6"/>
       <c r="G10" s="6"/>
-    </row>
-    <row r="11" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="21"/>
-      <c r="B11" s="24" t="s">
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="20"/>
+      <c r="B11" s="33" t="s">
+        <v>16</v>
+      </c>
+      <c r="C11" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="25"/>
-      <c r="D11" s="3"/>
+      <c r="D11" s="24"/>
       <c r="E11" s="3"/>
-      <c r="F11" s="5"/>
+      <c r="F11" s="3"/>
       <c r="G11" s="5"/>
-    </row>
-    <row r="12" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="21"/>
-      <c r="B12" s="7" t="s">
+      <c r="H11" s="5"/>
+    </row>
+    <row r="12" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="20"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="D12" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
-    </row>
-    <row r="13" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H12" s="3"/>
+    </row>
+    <row r="13" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="B13" s="10">
+      <c r="B13" s="31"/>
+      <c r="C13" s="10">
         <v>6.25E-2</v>
       </c>
-      <c r="C13" s="11">
+      <c r="D13" s="11">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D13" s="3"/>
       <c r="E13" s="3"/>
-      <c r="F13" s="4"/>
+      <c r="F13" s="3"/>
       <c r="G13" s="4"/>
-    </row>
-    <row r="14" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H13" s="4"/>
+    </row>
+    <row r="14" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B14" s="10">
+      <c r="B14" s="31"/>
+      <c r="C14" s="10">
         <v>6.25E-2</v>
       </c>
-      <c r="C14" s="11">
+      <c r="D14" s="11">
         <v>0.16666666666666666</v>
       </c>
-      <c r="D14" s="3"/>
       <c r="E14" s="3"/>
-      <c r="F14" s="4"/>
+      <c r="F14" s="3"/>
       <c r="G14" s="4"/>
-    </row>
-    <row r="15" spans="1:7" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="H14" s="4"/>
+    </row>
+    <row r="15" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="B15" s="10">
+      <c r="B15" s="31"/>
+      <c r="C15" s="10">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C15" s="11">
+      <c r="D15" s="11">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D15" s="3"/>
       <c r="E15" s="3"/>
-      <c r="F15" s="4"/>
+      <c r="F15" s="3"/>
       <c r="G15" s="4"/>
-    </row>
-    <row r="16" spans="1:7" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="12" t="s">
+      <c r="H15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="B16" s="10">
+      <c r="B16" s="32"/>
+      <c r="C16" s="10">
         <v>6.25E-2</v>
       </c>
-      <c r="C16" s="11">
+      <c r="D16" s="11">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
-    </row>
-    <row r="17" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="12" t="s">
+      <c r="H16" s="3"/>
+    </row>
+    <row r="17" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B17" s="10">
+      <c r="B17" s="32"/>
+      <c r="C17" s="10">
         <v>6.25E-2</v>
       </c>
-      <c r="C17" s="11">
+      <c r="D17" s="11">
         <v>0.125</v>
       </c>
-      <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
-    </row>
-    <row r="18" spans="1:10" ht="20.100000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A18" s="12" t="s">
+      <c r="H17" s="3"/>
+    </row>
+    <row r="18" spans="1:11" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B18" s="10">
+      <c r="B18" s="32"/>
+      <c r="C18" s="10">
         <v>8.3333333333333329E-2</v>
       </c>
-      <c r="C18" s="11">
+      <c r="D18" s="11">
         <v>0.1875</v>
       </c>
-      <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
       <c r="G18" s="3"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C19" s="1"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="C20" s="1"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="23"/>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H22" s="1"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H23" s="1"/>
-      <c r="I23" s="2"/>
+      <c r="H18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" s="36" customFormat="1" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="39" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="37">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D19" s="38">
+        <v>0.10416666666666667</v>
+      </c>
+      <c r="E19" s="35"/>
+      <c r="F19" s="35"/>
+      <c r="G19" s="35"/>
+      <c r="H19" s="35"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="D21" s="1"/>
+      <c r="J21" s="22"/>
+      <c r="K21" s="22"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I23" s="1"/>
       <c r="J23" s="2"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H24" s="1"/>
-      <c r="I24" s="2"/>
+      <c r="K23" s="2"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I24" s="1"/>
       <c r="J24" s="2"/>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="H25" s="1"/>
+      <c r="K24" s="2"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I25" s="1"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="2"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I26" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="A2:B2"/>
+  <mergeCells count="7">
+    <mergeCell ref="A2:C2"/>
     <mergeCell ref="A11:A12"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="I20:J20"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="A10:C10"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="J21:K21"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="B11:B12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967294" r:id="rId1"/>

</xml_diff>